<commit_message>
corrected god plate mistakes in yin and make changes easy
</commit_message>
<xml_diff>
--- a/qimen-earth.xlsx
+++ b/qimen-earth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GoogleDriveHoy\qimen-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1FE10B-CE4C-4944-A159-13672DF8C9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB4F45C-EF2B-4B71-B40D-FFD258B39515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34185" yWindow="1755" windowWidth="14400" windowHeight="13620" xr2:uid="{7A9BD3FF-F9D4-4EB7-9584-67CA3B29A2CF}"/>
+    <workbookView xWindow="3210" yWindow="3090" windowWidth="21600" windowHeight="11505" xr2:uid="{7A9BD3FF-F9D4-4EB7-9584-67CA3B29A2CF}"/>
   </bookViews>
   <sheets>
     <sheet name="地盤" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
     <t>離(S) 9</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>六十甲子</t>
+  </si>
+  <si>
+    <t>玄</t>
+  </si>
+  <si>
+    <t>虎</t>
   </si>
 </sst>
 </file>
@@ -353,7 +359,13 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>戊</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="2">
         <row r="1">
           <cell r="B1" t="str">
@@ -1967,7 +1979,7 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2039,7 @@
         <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2236,7 +2248,7 @@
         <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finished display day and time stem palace
</commit_message>
<xml_diff>
--- a/qimen-earth.xlsx
+++ b/qimen-earth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GoogleDriveHoy\qimen-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB4F45C-EF2B-4B71-B40D-FFD258B39515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B34625-04A3-4333-A882-C1C4D6FCE920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="3090" windowWidth="21600" windowHeight="11505" xr2:uid="{7A9BD3FF-F9D4-4EB7-9584-67CA3B29A2CF}"/>
+    <workbookView xWindow="31050" yWindow="2520" windowWidth="21600" windowHeight="11505" xr2:uid="{7A9BD3FF-F9D4-4EB7-9584-67CA3B29A2CF}"/>
   </bookViews>
   <sheets>
     <sheet name="地盤" sheetId="2" r:id="rId1"/>
@@ -1101,7 +1101,10 @@
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add 五行分析 fix chinese month sort
</commit_message>
<xml_diff>
--- a/qimen-earth.xlsx
+++ b/qimen-earth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GoogleDriveHoy\qimen-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B34625-04A3-4333-A882-C1C4D6FCE920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611B602A-3E80-47E6-B296-7E2DCB52F500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31050" yWindow="2520" windowWidth="21600" windowHeight="11505" xr2:uid="{7A9BD3FF-F9D4-4EB7-9584-67CA3B29A2CF}"/>
+    <workbookView xWindow="-25320" yWindow="330" windowWidth="25440" windowHeight="15540" xr2:uid="{7A9BD3FF-F9D4-4EB7-9584-67CA3B29A2CF}"/>
   </bookViews>
   <sheets>
     <sheet name="地盤" sheetId="2" r:id="rId1"/>
@@ -56,30 +56,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
-    <t>離(S) 9</t>
-  </si>
-  <si>
-    <t>巽(SE) 4</t>
-  </si>
-  <si>
-    <t>震(E) 3</t>
-  </si>
-  <si>
-    <t>艮(NE) 8</t>
-  </si>
-  <si>
-    <t>坎(N) 1</t>
-  </si>
-  <si>
-    <t>乾(NW) 6</t>
-  </si>
-  <si>
-    <t>兌(W) 7</t>
-  </si>
-  <si>
-    <t>坤(SW) 2</t>
-  </si>
-  <si>
     <t>減數</t>
   </si>
   <si>
@@ -258,6 +234,30 @@
   </si>
   <si>
     <t>虎</t>
+  </si>
+  <si>
+    <t>巽</t>
+  </si>
+  <si>
+    <t>震</t>
+  </si>
+  <si>
+    <t>艮</t>
+  </si>
+  <si>
+    <t>坎</t>
+  </si>
+  <si>
+    <t>乾</t>
+  </si>
+  <si>
+    <t>兌</t>
+  </si>
+  <si>
+    <t>坤</t>
+  </si>
+  <si>
+    <t>離</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1104,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,31 +1117,31 @@
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="Q1">
         <f>COLUMN()</f>
@@ -1913,60 +1913,60 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
         <v>9</v>
       </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" t="s">
-        <v>17</v>
-      </c>
       <c r="I26" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1992,86 +1992,86 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2080,28 +2080,28 @@
         <v>乙丑</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G4">
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2110,28 +2110,28 @@
         <v>丙寅</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2140,28 +2140,28 @@
         <v>丁卯</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2170,28 +2170,28 @@
         <v>戊辰</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2200,28 +2200,28 @@
         <v>己巳</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2230,28 +2230,28 @@
         <v>庚午</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G9">
         <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2260,13 +2260,13 @@
         <v>辛未</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2275,10 +2275,10 @@
         <v>壬申</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2287,15 +2287,15 @@
         <v>癸酉</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
@@ -2531,7 +2531,7 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>